<commit_message>
commited by sh May02 added config file
</commit_message>
<xml_diff>
--- a/utils/a.xlsx
+++ b/utils/a.xlsx
@@ -456,3200 +456,3200 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Marko</t>
+          <t>Elenise</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Vincent</t>
+          <t>Mendes</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>marko.vincent@example.com</t>
+          <t>elenise.mendes@example.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>079 838 19 71</t>
+          <t>(99) 9465-4183</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>beautifulmouse990</t>
+          <t>silverwolf633</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bosco1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Idunn</t>
+          <t>Dwight</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Gravem</t>
+          <t>Jackson</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>idunn.gravem@example.com</t>
+          <t>dwight.jackson@example.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>64649454</t>
+          <t>01-2098-0644</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>angryrabbit899</t>
+          <t>heavylion685</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>randy</t>
+          <t>rosario</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Elizabeth</t>
+          <t>Miranda</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Phillips</t>
+          <t>Leclercq</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>elizabeth.phillips@example.com</t>
+          <t>miranda.leclercq@example.com</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>041-604-3791</t>
+          <t>078 030 84 64</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>orangebutterfly274</t>
+          <t>whitegoose105</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>gggggg</t>
+          <t>colonial</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nurdan</t>
+          <t>Avery</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Yetkiner</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>nurdan.yetkiner@example.com</t>
+          <t>avery.davis@example.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>(487)-576-3679</t>
+          <t>015396 94567</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>orangepanda605</t>
+          <t>goldenelephant829</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>jazzman</t>
+          <t>floyd</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Angus</t>
+          <t>Toivo</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Tuomala</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>angus.white@example.com</t>
+          <t>toivo.tuomala@example.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>(076)-286-7419</t>
+          <t>04-603-333</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>angrytiger102</t>
+          <t>heavyfish839</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ranch</t>
+          <t>dogface</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Anette</t>
+          <t>Delores</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Van Miltenburg</t>
+          <t>Marshall</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>anette.vanmiltenburg@example.com</t>
+          <t>delores.marshall@example.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>(959)-873-4879</t>
+          <t>00-0016-4558</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>sadbear756</t>
+          <t>angryleopard627</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>chiquita</t>
+          <t>station</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Iris</t>
+          <t>Nicklas</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Selle</t>
+          <t>Christiansen</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>iris.selle@example.com</t>
+          <t>nicklas.christiansen@example.com</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0399-0925481</t>
+          <t>42658483</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>greenbird538</t>
+          <t>silverbutterfly214</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>goodbye</t>
+          <t>girls</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Alla</t>
+          <t>Alícia</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Radermacher</t>
+          <t>Rocha</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>alla.radermacher@example.com</t>
+          <t>alicia.rocha@example.com</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0579-7663107</t>
+          <t>(68) 5572-2343</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>heavyswan386</t>
+          <t>goldenfish735</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>logitech</t>
+          <t>forumwp</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Nils</t>
+          <t>Natalie</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Østerhus</t>
+          <t>Cunningham</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>nils.osterhus@example.com</t>
+          <t>natalie.cunningham@example.com</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>70480283</t>
+          <t>(106)-673-9257</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>redelephant308</t>
+          <t>ticklishkoala133</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>mian</t>
+          <t>fergie</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Milla</t>
+          <t>Dennis</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Salminen</t>
+          <t>Dufour</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>armyt.hydry@example.com</t>
+          <t>dennis.dufour@example.com</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>046-45959960</t>
+          <t>079 019 59 48</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>lazygorilla884</t>
+          <t>redelephant533</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>conan</t>
+          <t>cygnusx1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Tracy</t>
+          <t>Zoe</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Hill</t>
+          <t>Moore</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>tracy.hill@example.com</t>
+          <t>zoe.moore@example.com</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>01169 854395</t>
+          <t>(717)-727-7754</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>brownostrich711</t>
+          <t>yellowswan463</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>illini</t>
+          <t>teng</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Brett</t>
+          <t>Lillian</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Oliver</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>brett.washington@example.com</t>
+          <t>lillian.oliver@example.com</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>(239)-920-2516</t>
+          <t>016977 7965</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>browngorilla316</t>
+          <t>tinyelephant960</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>pluto</t>
+          <t>miller1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Elias</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Zhang</t>
+          <t>Larsen</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>john.zhang@example.com</t>
+          <t>elias.larsen@example.com</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>(524)-764-2436</t>
+          <t>88508824</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>silverpeacock265</t>
+          <t>ticklishmeercat275</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>leigh</t>
+          <t>building</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Guiseppe</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Hansen</t>
+          <t>Blanc</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>guiseppe.hansen@example.com</t>
+          <t>max.blanc@example.com</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0700-2000273</t>
+          <t>076 469 83 41</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>heavybear436</t>
+          <t>sadfrog658</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>dakota1</t>
+          <t>option</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Milla</t>
+          <t>Judy</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Salminen</t>
+          <t>Carpenter</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>mhmdth.prs@example.com</t>
+          <t>judy.carpenter@example.com</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>007-48623242</t>
+          <t>015394 32416</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>sadbutterfly278</t>
+          <t>blackswan852</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>rafael</t>
+          <t>compact</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Dawn</t>
+          <t>August</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Barnes</t>
+          <t>Johansen</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>dawn.barnes@example.com</t>
+          <t>august.johansen@example.com</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>02-8517-0783</t>
+          <t>08419440</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>yellowgorilla996</t>
+          <t>goldenbird842</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>nation</t>
+          <t>india</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Glória</t>
+          <t>Nataniel</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Freitas</t>
+          <t>Leidland</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>gloria.freitas@example.com</t>
+          <t>nataniel.leidland@example.com</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>(08) 7004-4033</t>
+          <t>21559278</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>redwolf852</t>
+          <t>bluepeacock644</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>marisa</t>
+          <t>surprise</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Frida</t>
+          <t>Jeffrey</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Andersen</t>
+          <t>Oliver</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>frida.andersen@example.com</t>
+          <t>jeffrey.oliver@example.com</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>29336799</t>
+          <t>00-2968-4691</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>purplebutterfly283</t>
+          <t>redelephant821</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>aztnm</t>
+          <t>badman</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Gül</t>
+          <t>Philipp</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ertepınar</t>
+          <t>Francois</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>gul.ertepinar@example.com</t>
+          <t>philipp.francois@example.com</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>(252)-748-2355</t>
+          <t>075 561 17 58</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>silvermeercat463</t>
+          <t>blackelephant591</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>holycow</t>
+          <t>alyssa</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Amy</t>
+          <t>Laura</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Kristensen</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>amy.young@example.com</t>
+          <t>laura.kristensen@example.com</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>015396 13678</t>
+          <t>76170045</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>yellowmeercat666</t>
+          <t>sadduck923</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>polo</t>
+          <t>skate</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>William</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>da Mata</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>william.jones@example.com</t>
+          <t>lucas.damata@example.com</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>(514)-694-6036</t>
+          <t>(22) 8035-7112</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>blackladybug402</t>
+          <t>brownrabbit124</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>dirtbike</t>
+          <t>rockhard</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Okan</t>
+          <t>Nelli</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Evliyaoğlu</t>
+          <t>Niva</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>okan.evliyaoglu@example.com</t>
+          <t>nelli.niva@example.com</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>(240)-234-8189</t>
+          <t>07-243-715</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>happybird137</t>
+          <t>smallkoala445</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>sandy</t>
+          <t>torpedo</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Sofia</t>
+          <t>Aurora</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Nielsen</t>
+          <t>Diaz</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>sofia.nielsen@example.com</t>
+          <t>aurora.diaz@example.com</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>68439016</t>
+          <t>919-706-534</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>ticklishduck511</t>
+          <t>angrypanda505</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>phillies</t>
+          <t>1227</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Jose</t>
+          <t>Jimmie</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Obrien</t>
+          <t>Harrison</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>jose.obrien@example.com</t>
+          <t>jimmie.harrison@example.com</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>(353)-025-4883</t>
+          <t>016974 90853</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>redladybug761</t>
+          <t>happycat935</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>clapton</t>
+          <t>janet</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Oona</t>
+          <t>Jordano</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Halonen</t>
+          <t>Moraes</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>oona.halonen@example.com</t>
+          <t>jordano.moraes@example.com</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>07-454-156</t>
+          <t>(07) 2539-1231</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>smalllion164</t>
+          <t>blackelephant429</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>beatrice</t>
+          <t>concrete</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Yasemin</t>
+          <t>Åsmund</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Kavaklıoğlu</t>
+          <t>Meier</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>yasemin.kavaklioglu@example.com</t>
+          <t>asmund.meier@example.com</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>(625)-665-4141</t>
+          <t>54749514</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>lazypeacock353</t>
+          <t>angrymeercat920</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>guest</t>
+          <t>chavez</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Johnni</t>
+          <t>Deanna</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Pierce</t>
+          <t>Richardson</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>johnni.pierce@example.com</t>
+          <t>deanna.richardson@example.com</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>071-623-7396</t>
+          <t>09-8281-3387</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>yellowzebra650</t>
+          <t>orangedog955</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>susanne</t>
+          <t>scorpio1</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Elmer</t>
+          <t>Ytsje</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Riley</t>
+          <t>Nederpel</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>elmer.riley@example.com</t>
+          <t>ytsje.nederpel@example.com</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>015394 95914</t>
+          <t>(981)-745-4898</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>purplecat726</t>
+          <t>blueostrich580</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>676767</t>
+          <t>rusty2</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Nelli</t>
+          <t>Mato</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Aalto</t>
+          <t>Kurz</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>nelli.aalto@example.com</t>
+          <t>mato.kurz@example.com</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>07-594-418</t>
+          <t>0371-6885531</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>silverleopard766</t>
+          <t>goldentiger952</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>wordpass</t>
+          <t>redsox1</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Ege</t>
+          <t>Byron</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Solmaz</t>
+          <t>Price</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ege.solmaz@example.com</t>
+          <t>byron.price@example.com</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>(798)-046-4825</t>
+          <t>021-453-1593</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>beautifulpeacock260</t>
+          <t>brownlion766</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>closer</t>
+          <t>585858</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Andre</t>
+          <t>Joan</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Kober</t>
+          <t>Mason</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>andre.kober@example.com</t>
+          <t>joan.mason@example.com</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0602-3592719</t>
+          <t>(757)-339-5410</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>bluewolf374</t>
+          <t>smallzebra446</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>salvador</t>
+          <t>mexican</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Kamile</t>
+          <t>Maël</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Valstad</t>
+          <t>Mathieu</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>kamile.valstad@example.com</t>
+          <t>sm.glshn@example.com</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>22901410</t>
+          <t>072-20484499</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>goldenbird745</t>
+          <t>crazyelephant764</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>godfather</t>
+          <t>5678</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Rosita</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Santos</t>
+          <t>Andrews</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>rosita.santos@example.com</t>
+          <t>diana.andrews@example.com</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>(81) 6474-3306</t>
+          <t>041-579-5408</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>sadwolf793</t>
+          <t>purpleswan977</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>qwert40</t>
+          <t>woody</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Clinton</t>
+          <t>Astrid</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Reynolds</t>
+          <t>Christiansen</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>clinton.reynolds@example.com</t>
+          <t>astrid.christiansen@example.com</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>02-2229-4533</t>
+          <t>24802178</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>crazypanda776</t>
+          <t>ticklishpeacock437</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>glennwei</t>
+          <t>good</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Amelia</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Gautier</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>amelia.gautier@example.com</t>
+          <t>max.williams@example.com</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>03-24-75-17-70</t>
+          <t>(324)-280-0760</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>lazydog589</t>
+          <t>redleopard948</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>blabla</t>
+          <t>peter1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Mikkel</t>
+          <t>Raymond</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Larsen</t>
+          <t>Arnaud</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>mikkel.larsen@example.com</t>
+          <t>raymond.arnaud@example.com</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>47939838</t>
+          <t>079 940 01 63</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>bigladybug822</t>
+          <t>beautifulmeercat443</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>birthday</t>
+          <t>gabby</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Alfonso</t>
+          <t>Laly</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Vega</t>
+          <t>Clement</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>alfonso.vega@example.com</t>
+          <t>laly.clement@example.com</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>964-985-087</t>
+          <t>01-10-48-92-84</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>sadwolf970</t>
+          <t>yellowsnake468</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>truck1</t>
+          <t>timeout</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Avery</t>
+          <t>Jeremy</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Campbell</t>
+          <t>Stone</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>avery.campbell@example.com</t>
+          <t>jeremy.stone@example.com</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>313-361-5686</t>
+          <t>(502)-252-6529</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>orangekoala696</t>
+          <t>crazyzebra421</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>dalshe</t>
+          <t>santiago</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Francisco de Borja</t>
+          <t>Carlos</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Silveira</t>
+          <t>Mendez</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>franciscodeborja.silveira@example.com</t>
+          <t>carlos.mendez@example.com</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>(57) 6752-6558</t>
+          <t>928-700-169</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>ticklishfish595</t>
+          <t>purplekoala396</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>chopin</t>
+          <t>flash</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Milla</t>
+          <t>Edward</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Salminen</t>
+          <t>Taylor</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>mrym.ysmy@example.com</t>
+          <t>edward.taylor@example.com</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>058-66470172</t>
+          <t>(243)-964-6320</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>blackelephant909</t>
+          <t>lazydog628</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>streaming</t>
+          <t>evolutio</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Adriana</t>
+          <t>Ege</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Gallardo</t>
+          <t>Nalbantoğlu</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>adriana.gallardo@example.com</t>
+          <t>ege.nalbantoglu@example.com</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>963-725-351</t>
+          <t>(162)-244-4557</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>bluekoala610</t>
+          <t>whiteladybug435</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>bruce1</t>
+          <t>hakr</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Ardian</t>
+          <t>June</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Michel</t>
+          <t>Lane</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ardian.michel@example.com</t>
+          <t>june.lane@example.com</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>078 687 71 00</t>
+          <t>(004)-360-9366</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>smallsnake888</t>
+          <t>goldensnake696</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>1234567</t>
+          <t>fingers</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Freya</t>
+          <t>Rafael</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Thomas</t>
+          <t>Turner</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>freya.thomas@example.com</t>
+          <t>rafael.turner@example.com</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>(559)-209-9486</t>
+          <t>021-739-4072</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>ticklishgorilla384</t>
+          <t>whitebutterfly857</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>camero</t>
+          <t>diablo</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Milja</t>
+          <t>Onni</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Kyllo</t>
+          <t>Toivonen</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>milja.kyllo@example.com</t>
+          <t>onni.toivonen@example.com</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>08-542-192</t>
+          <t>02-847-121</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>beautifulfrog206</t>
+          <t>heavypeacock868</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>bookie</t>
+          <t>pasadena</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Juliette</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Carpenter</t>
+          <t>Ambrose</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>diane.carpenter@example.com</t>
+          <t>juliette.ambrose@example.com</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>071-181-5598</t>
+          <t>398-371-6953</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>purpleladybug662</t>
+          <t>bigtiger887</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>millwall</t>
+          <t>cattle</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Seleni</t>
+          <t>Hasan</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Cavalcanti</t>
+          <t>Uhlig</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>seleni.cavalcanti@example.com</t>
+          <t>hasan.uhlig@example.com</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>(29) 2515-1771</t>
+          <t>0110-7408570</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>redmeercat747</t>
+          <t>purplerabbit480</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>martin1</t>
+          <t>corvette</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Caroline</t>
+          <t>Veera</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Rasmussen</t>
+          <t>Sippola</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>caroline.rasmussen@example.com</t>
+          <t>veera.sippola@example.com</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>03776423</t>
+          <t>03-336-263</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>yellowfish950</t>
+          <t>blackmeercat874</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>iforgot</t>
+          <t>zappa</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Suzanne</t>
+          <t>Hannah</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Turner</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>suzanne.turner@example.com</t>
+          <t>hannah.brown@example.com</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>02-2952-3361</t>
+          <t>918-539-1032</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>brownleopard250</t>
+          <t>silverfrog192</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>bomb</t>
+          <t>753951</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Rosalyn</t>
+          <t>Ethan</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Rubingh</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>rosalyn.russell@example.com</t>
+          <t>ethan.rubingh@example.com</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>041-904-4781</t>
+          <t>(517)-081-4790</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>purplebird625</t>
+          <t>angryfrog601</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>bingo1</t>
+          <t>bryan1</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Leta</t>
+          <t>Tiffany</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Cooper</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>leta.james@example.com</t>
+          <t>tiffany.cooper@example.com</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>(839)-745-2288</t>
+          <t>00-5315-4042</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>sadmouse411</t>
+          <t>orangeduck403</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>defense</t>
+          <t>757575</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Gökhan</t>
+          <t>Victoire</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Tokgöz</t>
+          <t>Giraud</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>gokhan.tokgoz@example.com</t>
+          <t>victoire.giraud@example.com</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>(902)-129-1779</t>
+          <t>02-56-16-88-34</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>smallelephant811</t>
+          <t>bluecat552</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>cheese</t>
+          <t>knight1</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Villads</t>
+          <t>Sanna</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Jensen</t>
+          <t>Molde</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>villads.jensen@example.com</t>
+          <t>sanna.molde@example.com</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>60185744</t>
+          <t>36003483</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>silverladybug945</t>
+          <t>goldenwolf673</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>shaolin</t>
+          <t>tetsuo</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Linn</t>
+          <t>Charlie</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Herland</t>
+          <t>Morin</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>linn.herland@example.com</t>
+          <t>charlie.morin@example.com</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>75532704</t>
+          <t>008-932-6048</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>tinybear967</t>
+          <t>silverleopard449</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>donovan</t>
+          <t>mnbvcx</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Edir</t>
+          <t>Mariano</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>da Rocha</t>
+          <t>Morales</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>edir.darocha@example.com</t>
+          <t>mariano.morales@example.com</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>(72) 8692-0824</t>
+          <t>981-228-036</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>browntiger199</t>
+          <t>purplesnake385</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>mmmmmmmm</t>
+          <t>nurses</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Adam</t>
+          <t>Batur</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Sanchez</t>
+          <t>Dağdaş</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>adam.sanchez@example.com</t>
+          <t>batur.dagdas@example.com</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>03-10-02-89-00</t>
+          <t>(802)-074-1864</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>smallpanda921</t>
+          <t>blackgoose678</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>babyface</t>
+          <t>astrid</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Dustin</t>
+          <t>Ali</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Walker</t>
+          <t>Overdijk</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>dustin.walker@example.com</t>
+          <t>ali.overdijk@example.com</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>(935)-124-2786</t>
+          <t>(451)-383-3549</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>organiczebra183</t>
+          <t>happyleopard133</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>lightnin</t>
+          <t>chase</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Alizee</t>
+          <t>Brede</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Da Silva</t>
+          <t>Bruvik</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>alizee.dasilva@example.com</t>
+          <t>brede.bruvik@example.com</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>03-22-32-60-60</t>
+          <t>71111134</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>whitemeercat162</t>
+          <t>silverswan286</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>juggalo</t>
+          <t>cheyenne</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Violet</t>
+          <t>Oliver</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Walker</t>
+          <t>Schie</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>violet.walker@example.com</t>
+          <t>oliver.schie@example.com</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>(107)-848-8696</t>
+          <t>34197210</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>organiccat670</t>
+          <t>silverladybug825</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>spanner</t>
+          <t>nicola</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Linda</t>
+          <t>Mikaela</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Cole</t>
+          <t>Sparby</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>linda.cole@example.com</t>
+          <t>mikaela.sparby@example.com</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>016973 07863</t>
+          <t>22480290</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>blackleopard307</t>
+          <t>yellowwolf781</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>socks</t>
+          <t>rockhard</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Mélanie</t>
+          <t>Bella</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Lefebvre</t>
+          <t>Ræstad</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>melanie.lefebvre@example.com</t>
+          <t>bella.raestad@example.com</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>077 872 22 67</t>
+          <t>84767654</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>whitefish519</t>
+          <t>angryzebra296</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>147258</t>
+          <t>syzygy</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Isaac</t>
+          <t>Maël</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Nordli</t>
+          <t>Mathieu</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>isaac.nordli@example.com</t>
+          <t>ary.khmrw@example.com</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>54470088</t>
+          <t>003-95432384</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>happypeacock630</t>
+          <t>organicelephant874</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>trident</t>
+          <t>wave</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Pinja</t>
+          <t>Stephanie</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Korpela</t>
+          <t>Gardner</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>pinja.korpela@example.com</t>
+          <t>stephanie.gardner@example.com</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>09-670-783</t>
+          <t>(753)-860-1980</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>smallcat802</t>
+          <t>sadtiger883</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>sheba1</t>
+          <t>callisto</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Mustafa</t>
+          <t>Dylan</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Pektemek</t>
+          <t>Gauthier</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>mustafa.pektemek@example.com</t>
+          <t>dylan.gauthier@example.com</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>(782)-473-8145</t>
+          <t>686-839-0419</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>purplefrog728</t>
+          <t>yellowlion450</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>snowboard</t>
+          <t>10101010</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Bastien</t>
+          <t>Aubrey</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Renard</t>
+          <t>Richards</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>bastien.renard@example.com</t>
+          <t>aubrey.richards@example.com</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>076 333 83 17</t>
+          <t>(403)-945-0160</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>yellowgorilla785</t>
+          <t>greenladybug907</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>irish1</t>
+          <t>bluedog</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>Storm</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Rautio</t>
+          <t>Petersen</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>emma.rautio@example.com</t>
+          <t>storm.petersen@example.com</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>06-157-059</t>
+          <t>53193592</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>angrypeacock123</t>
+          <t>angryostrich913</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>stinker</t>
+          <t>lucifer</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Désirée</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Barbier</t>
+          <t>Ruiz</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>desiree.barbier@example.com</t>
+          <t>linda.ruiz@example.com</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>075 787 15 49</t>
+          <t>(772)-782-2427</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>angrypanda342</t>
+          <t>happygorilla617</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>wood</t>
+          <t>bartman</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Ezio</t>
+          <t>Victoria</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Martinez</t>
+          <t>Soto</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>ezio.martinez@example.com</t>
+          <t>victoria.soto@example.com</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>02-05-04-31-39</t>
+          <t>021-991-8946</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>organicgorilla170</t>
+          <t>crazymouse453</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>musica</t>
+          <t>lowell</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Milla</t>
+          <t>Victoria</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Salminen</t>
+          <t>Ramos</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>dyn.sdr@example.com</t>
+          <t>victoria.ramos@example.com</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>032-48890714</t>
+          <t>(742)-075-9522</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>whitesnake641</t>
+          <t>organicmeercat901</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>reggie</t>
+          <t>hithere</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Haije</t>
+          <t>Derek</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Obdam</t>
+          <t>Payne</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>haije.obdam@example.com</t>
+          <t>derek.payne@example.com</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>(618)-156-1204</t>
+          <t>(665)-196-5646</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>brownsnake103</t>
+          <t>bluetiger706</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>riddle</t>
+          <t>bread</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Emmie</t>
+          <t>Sofia</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Dupont</t>
+          <t>Andersen</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>emmie.dupont@example.com</t>
+          <t>sofia.andersen@example.com</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>05-47-95-43-20</t>
+          <t>84927820</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>beautifulrabbit889</t>
+          <t>purplewolf221</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>master1</t>
+          <t>traveler</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Ülkü</t>
+          <t>Gonca</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Çevik</t>
+          <t>Abanuz</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>ulku.cevik@example.com</t>
+          <t>gonca.abanuz@example.com</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>(526)-731-9692</t>
+          <t>(758)-633-9621</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>brownzebra408</t>
+          <t>beautifulswan638</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>lemons</t>
+          <t>google</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Karen</t>
+          <t>George</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Weaver</t>
+          <t>Young</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>karen.weaver@example.com</t>
+          <t>george.young@example.com</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>019467 37786</t>
+          <t>08-1863-3300</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>greengoose705</t>
+          <t>angrygorilla879</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>andrews</t>
+          <t>toonarmy</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Milla</t>
+          <t>Filippo</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Salminen</t>
+          <t>Meyer</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>swgnd.khwty@example.com</t>
+          <t>filippo.meyer@example.com</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>068-07868421</t>
+          <t>077 896 15 32</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>beautifulmouse540</t>
+          <t>sadpeacock170</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>lakers</t>
+          <t>robotics</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Étienne</t>
+          <t>Inmaculada</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Fournier</t>
+          <t>Reyes</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>etienne.fournier@example.com</t>
+          <t>inmaculada.reyes@example.com</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>075 915 96 96</t>
+          <t>903-439-926</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>yellowzebra569</t>
+          <t>smallfish866</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>dallas1</t>
+          <t>boston1</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Milla</t>
+          <t>Jake</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Salminen</t>
+          <t>Zhang</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>pry.ysmy@example.com</t>
+          <t>jake.zhang@example.com</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>090-42085066</t>
+          <t>(561)-156-1558</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>happymeercat518</t>
+          <t>sadbird507</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>freee</t>
+          <t>diva</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Stella</t>
+          <t>Polle</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Barbier</t>
+          <t>De Beijer</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>stella.barbier@example.com</t>
+          <t>polle.debeijer@example.com</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>04-10-31-10-76</t>
+          <t>(911)-557-0700</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>bigmeercat189</t>
+          <t>lazyswan979</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>blanco</t>
+          <t>margie</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Cory</t>
+          <t>Poppy</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Sims</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>cory.sims@example.com</t>
+          <t>poppy.martin@example.com</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>(239)-330-8455</t>
+          <t>(695)-456-6982</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>blackduck251</t>
+          <t>brownfish417</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>dinosaur</t>
+          <t>benny</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Alicia</t>
+          <t>Kristiane</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Legrand</t>
+          <t>Furuhaug</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>alicia.legrand@example.com</t>
+          <t>kristiane.furuhaug@example.com</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>076 253 85 12</t>
+          <t>61915205</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>whitewolf669</t>
+          <t>ticklishduck190</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>manson</t>
+          <t>moose1</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Mustafa</t>
+          <t>Rica</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Hegg</t>
+          <t>Almeida</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>mustafa.hegg@example.com</t>
+          <t>rica.almeida@example.com</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>28370112</t>
+          <t>(38) 3641-9800</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>smallcat766</t>
+          <t>sadzebra761</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>stars</t>
+          <t>thegreat</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Ida</t>
+          <t>Cristobal</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Jensen</t>
+          <t>Morales</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>ida.jensen@example.com</t>
+          <t>cristobal.morales@example.com</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>43897518</t>
+          <t>928-045-907</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>ticklishbutterfly795</t>
+          <t>whitebutterfly550</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>987456</t>
+          <t>lloyd</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Katarina</t>
+          <t>Heather</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Hellwig</t>
+          <t>Mccoy</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>katarina.hellwig@example.com</t>
+          <t>heather.mccoy@example.com</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>0411-0099201</t>
+          <t>016977 94107</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>crazybird575</t>
+          <t>smalltiger797</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>christi</t>
+          <t>baggins</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Victoria</t>
+          <t>Melodie</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Poulsen</t>
+          <t>Lam</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>victoria.poulsen@example.com</t>
+          <t>melodie.lam@example.com</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>69578790</t>
+          <t>255-608-1351</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>bigrabbit794</t>
+          <t>brownfish438</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>qwerty</t>
+          <t>puppy</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Fabiana</t>
+          <t>Océane</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Leclerc</t>
+          <t>Moreau</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>fabiana.leclerc@example.com</t>
+          <t>oceane.moreau@example.com</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>079 137 48 37</t>
+          <t>03-12-20-76-37</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>tinyfrog434</t>
+          <t>happypanda851</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>hardon</t>
+          <t>marine</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Sophie</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Rivera</t>
+          <t>Carlson</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>sophie.rivera@example.com</t>
+          <t>russell.carlson@example.com</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>01055 30820</t>
+          <t>(541)-257-2839</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>organicwolf858</t>
+          <t>blueelephant658</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>storm1</t>
+          <t>getout</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>Solène</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Herrera</t>
+          <t>Henry</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>martin.herrera@example.com</t>
+          <t>solene.henry@example.com</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>989-797-625</t>
+          <t>03-75-03-50-75</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>beautifulgoose120</t>
+          <t>silverlion409</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>capslock</t>
+          <t>buzz</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Barbara</t>
+          <t>Pirmin</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Mcdonalid</t>
+          <t>Petit</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>barbara.mcdonalid@example.com</t>
+          <t>pirmin.petit@example.com</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>0101 193 7690</t>
+          <t>075 344 01 05</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>sadbird200</t>
+          <t>blueostrich666</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>gorgeous</t>
+          <t>gangster</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Milla</t>
+          <t>Maël</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Salminen</t>
+          <t>Mathieu</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>hsty.rdyyn@example.com</t>
+          <t>myraaly.sdr@example.com</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>077-02595796</t>
+          <t>059-22394198</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>angrycat660</t>
+          <t>greenwolf998</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>xiao</t>
+          <t>montana</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Xavier</t>
+          <t>Terry</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Novak</t>
+          <t>Verton</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>xavier.novak@example.com</t>
+          <t>terry.verton@example.com</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>589-319-9097</t>
+          <t>(216)-835-1704</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>crazyswan500</t>
+          <t>tinygoose979</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>tootsie</t>
+          <t>judy</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Halbe</t>
+          <t>Adem</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Ter Bruggen</t>
+          <t>Çamdalı</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>halbe.terbruggen@example.com</t>
+          <t>adem.camdali@example.com</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>(054)-595-8716</t>
+          <t>(517)-545-1848</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>crazybird200</t>
+          <t>heavyfrog195</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>turtle</t>
+          <t>12345a</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Layla</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Romero</t>
+          <t>Rodriquez</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>patrick.romero@example.com</t>
+          <t>layla.rodriquez@example.com</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>016977 26862</t>
+          <t>01-1986-2244</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>sadlion549</t>
+          <t>bigsnake864</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>cowboys</t>
+          <t>history</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Ron</t>
+          <t>Lorenzo</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Gray</t>
+          <t>Dupont</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>ron.gray@example.com</t>
+          <t>lorenzo.dupont@example.com</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>071-995-9850</t>
+          <t>03-64-02-66-29</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>brownpanda787</t>
+          <t>ticklishduck534</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>dumb</t>
+          <t>151515</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Beau</t>
+          <t>Alisa</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Mattila</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>beau.johnson@example.com</t>
+          <t>alisa.mattila@example.com</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>(298)-199-9442</t>
+          <t>04-819-728</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>blackswan774</t>
+          <t>heavydog548</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>porter</t>
+          <t>mistress</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Giuliana</t>
+          <t>Ella</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Moulin</t>
+          <t>Walters</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>giuliana.moulin@example.com</t>
+          <t>ella.walters@example.com</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>075 494 46 64</t>
+          <t>(313)-157-7441</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>heavyelephant110</t>
+          <t>organicgorilla845</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>passwor1</t>
+          <t>internet</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Luis</t>
+          <t>Sam</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Payne</t>
+          <t>Graham</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>luis.payne@example.com</t>
+          <t>sam.graham@example.com</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>(980)-946-1426</t>
+          <t>01930 60833</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>blackfish470</t>
+          <t>sadleopard702</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>loud</t>
+          <t>mclaren</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Lea</t>
+          <t>Saana</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Gauthier</t>
+          <t>Heikkinen</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>lea.gauthier@example.com</t>
+          <t>saana.heikkinen@example.com</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>659-163-9039</t>
+          <t>09-597-283</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>ticklishdog587</t>
+          <t>crazylion786</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>macross</t>
+          <t>millions</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Edward</t>
+          <t>Lizzy</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Walters</t>
+          <t>Van de Hoef</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>edward.walters@example.com</t>
+          <t>lizzy.vandehoef@example.com</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>061-797-4346</t>
+          <t>(101)-444-9855</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>redmouse419</t>
+          <t>heavylion975</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>letsgo</t>
+          <t>lolo</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Vicky</t>
+          <t>Rebecca</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Mitchell</t>
+          <t>Simpson</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>vicky.mitchell@example.com</t>
+          <t>rebecca.simpson@example.com</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>041-728-1016</t>
+          <t>019467 59060</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>angrycat883</t>
+          <t>blackelephant305</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>impala</t>
+          <t>brendan</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Markus</t>
+          <t>Annabelle</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Leroy</t>
+          <t>Ouellet</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>markus.leroy@example.com</t>
+          <t>annabelle.ouellet@example.com</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>075 754 69 92</t>
+          <t>416-161-5834</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>smallfish333</t>
+          <t>silverbird981</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>standard</t>
+          <t>escape</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Faber</t>
+          <t>Joshua</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Biesheuvel</t>
+          <t>Martinez</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>faber.biesheuvel@example.com</t>
+          <t>joshua.martinez@example.com</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>(259)-682-3712</t>
+          <t>041-746-1578</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>tinypanda405</t>
+          <t>yellowcat635</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>nwo4life</t>
+          <t>chess</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Edward</t>
+          <t>Ricardo</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Robinson</t>
+          <t>Dahm</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>edward.robinson@example.com</t>
+          <t>ricardo.dahm@example.com</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>011-805-1221</t>
+          <t>0765-6692902</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>beautifulgorilla108</t>
+          <t>brownpanda963</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>951753</t>
+          <t>domain</t>
         </is>
       </c>
     </row>

</xml_diff>